<commit_message>
Extended the measurment and scale
</commit_message>
<xml_diff>
--- a/reports/measurement_scale.xlsx
+++ b/reports/measurement_scale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliasgarov\Documents\Workspace\University\Guided Research I\Repo\guidedresearchproject-aliasgerovs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6442E3D4-9195-414D-8715-C22479A5CB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907B0E46-75F9-4F79-8261-59C3E1262091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{42017D82-C666-4BCD-9F4A-24A5728EA3AA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>number_of_clients</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>learning_rate</t>
+  </si>
+  <si>
+    <t>Number of training epochs</t>
+  </si>
+  <si>
+    <t>batch size</t>
+  </si>
+  <si>
+    <t>Momentum</t>
   </si>
 </sst>
 </file>
@@ -55,15 +64,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +86,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,6 +887,706 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Classification model accuracy vs number of epochs</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$40:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$40:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.95840000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96030000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9647</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9637</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96140000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A194-48BD-876B-8CD20DA0B037}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="860485952"/>
+        <c:axId val="1071152112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="860485952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1071152112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1071152112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="860485952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Classification model accuracy vs batch size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$55:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$55:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.96140000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96120000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78120000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB75-434C-8986-22D3C328AC8D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="615149423"/>
+        <c:axId val="818641855"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="615149423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818641855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="818641855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="615149423"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -938,6 +1667,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1455,6 +2264,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2044,7 +3885,134 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D70540D-DB14-4EA1-A247-FD5A45CF03A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>434974</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC4E7A1-FA3C-4DB4-AC7B-05F20C14DDAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E967411C-BB2A-4AD3-A1CD-EFC0BE02FAB4}" name="Table1" displayName="Table1" ref="A54:B57" totalsRowShown="0">
+  <autoFilter ref="A54:B57" xr:uid="{C164F9E1-FB9D-438C-B3C9-FDE0B2BB0CC1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C9BFB60F-88E6-45CA-A4CD-BDD8C7AAD240}" name="batch size"/>
+    <tableColumn id="2" xr3:uid="{A9EEF5F2-00FF-46A2-AF74-B0E376751CAB}" name="accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D3E10690-649C-493D-979B-661557186F3B}" name="Table2" displayName="Table2" ref="A1:B9" totalsRowShown="0">
+  <autoFilter ref="A1:B9" xr:uid="{64E57CBA-5712-4009-931E-091BDD35ED9F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D7679BC9-8C2B-4BFD-B0D2-CB941FFA2F42}" name="number_of_clients"/>
+    <tableColumn id="2" xr3:uid="{342DAF14-BA14-430B-8579-22C37B7BB9E2}" name="accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7AF6B39A-456B-47B2-BA34-D25508277493}" name="Table3" displayName="Table3" ref="A22:B29" totalsRowShown="0">
+  <autoFilter ref="A22:B29" xr:uid="{537C3016-80EC-4751-B32F-A312D9398FF2}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0059E049-F345-4248-B2C7-AECBC1A0D3FC}" name="learning_rate"/>
+    <tableColumn id="2" xr3:uid="{C3361D01-9343-428F-8624-355A87330A70}" name="accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85C7EA50-B361-4847-B23E-930A98005AF1}" name="Table4" displayName="Table4" ref="A39:B45" totalsRowShown="0">
+  <autoFilter ref="A39:B45" xr:uid="{15400424-0B90-4A90-AA3A-852C57B2A0FE}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CD2748C3-B54A-4A51-872C-E254633B8590}" name="Number of training epochs"/>
+    <tableColumn id="2" xr3:uid="{25CCB545-5656-42DA-99D5-A37FF8DCBB8B}" name="accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EF9C47D8-B157-4A66-A9E5-DD2B2CFAC4AC}" name="Table5" displayName="Table5" ref="A74:B78" totalsRowShown="0">
+  <autoFilter ref="A74:B78" xr:uid="{448B4242-19F8-46B9-943B-9D8A08881926}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4C484FF3-311E-42A9-BE24-CBD58089A373}" name="Momentum"/>
+    <tableColumn id="2" xr3:uid="{FD144FFF-8723-4FC2-99A8-E9B1852FDCAB}" name="accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2344,15 +4312,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2851543B-2CEF-4758-A632-6B06205C0621}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -2491,9 +4460,141 @@
         <v>0.96030000000000004</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.95840000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>0.96030000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>0.96250000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>0.9647</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>25</v>
+      </c>
+      <c r="B44">
+        <v>0.9637</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>30</v>
+      </c>
+      <c r="B45">
+        <v>0.96140000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>64</v>
+      </c>
+      <c r="B55">
+        <v>0.96140000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>32</v>
+      </c>
+      <c r="B56">
+        <v>0.96120000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>16</v>
+      </c>
+      <c r="B57">
+        <v>0.78120000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>0.8</v>
+      </c>
+      <c r="B75" s="1">
+        <v>0.96140000000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>0.6</v>
+      </c>
+      <c r="B76">
+        <v>0.95720000000000005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>0.4</v>
+      </c>
+      <c r="B77">
+        <v>0.95409999999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="5">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Momentum dependencies has been added
</commit_message>
<xml_diff>
--- a/reports/measurement_scale.xlsx
+++ b/reports/measurement_scale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliasgarov\Documents\Workspace\University\Guided Research I\Repo\guidedresearchproject-aliasgerovs\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907B0E46-75F9-4F79-8261-59C3E1262091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E56084-FE1B-4AFD-8AA4-1AED3AEB48F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{42017D82-C666-4BCD-9F4A-24A5728EA3AA}"/>
   </bookViews>
@@ -3816,15 +3816,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>511174</xdr:colOff>
+      <xdr:colOff>511175</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>22224</xdr:rowOff>
+      <xdr:rowOff>22225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>63499</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>88899</xdr:rowOff>
+      <xdr:colOff>25401</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3853,13 +3853,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>479424</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>3174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>603249</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>184149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3889,14 +3889,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3924,15 +3924,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>434974</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>492124</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>50799</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>158749</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4314,8 +4314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2851543B-2CEF-4758-A632-6B06205C0621}">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>